<commit_message>
Research project page updated and navbar and footer integrated
</commit_message>
<xml_diff>
--- a/CSPIT_Ongoing.Projects_Till.date.1.xlsx
+++ b/CSPIT_Ongoing.Projects_Till.date.1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Website\Research_Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4518248c6cd0c0d5/Desktop/CSPIT_NEW_2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_4C39D39E909098698551CDA3F85D8D6F0A8693F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3A5036C-0E14-462B-A29A-D46CE76C9695}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectListing" sheetId="1" r:id="rId1"/>
@@ -1527,8 +1528,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2481,64 +2482,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="W1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.8984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.09765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.69921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.8984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.8984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36.296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="36.296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.8984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="33.69921875" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="36.296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.796875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.09765625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="36.296875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="43" max="45" width="36.296875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.296875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="36.296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="45" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="1" customFormat="1" ht="9.6">
+    <row r="1" spans="1:49" s="1" customFormat="1" ht="9.6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2591,7 +2592,7 @@
       <c r="AV1" s="8"/>
       <c r="AW1" s="9"/>
     </row>
-    <row r="2" spans="1:49" s="2" customFormat="1" ht="13.2">
+    <row r="2" spans="1:49" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:49" s="4" customFormat="1" ht="72.599999999999994">
+    <row r="3" spans="1:49" s="4" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:49" s="4" customFormat="1" ht="59.4">
+    <row r="4" spans="1:49" s="4" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:49" s="4" customFormat="1" ht="118.8">
+    <row r="5" spans="1:49" s="4" customFormat="1" ht="125.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -3187,7 +3188,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:49" s="4" customFormat="1" ht="145.19999999999999">
+    <row r="6" spans="1:49" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:49" s="4" customFormat="1" ht="26.4">
+    <row r="7" spans="1:49" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -3485,7 +3486,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:49" s="4" customFormat="1" ht="13.2">
+    <row r="8" spans="1:49" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -3634,7 +3635,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:49" s="4" customFormat="1" ht="132">
+    <row r="9" spans="1:49" s="4" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -3783,7 +3784,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:49" s="4" customFormat="1" ht="105.6">
+    <row r="10" spans="1:49" s="4" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -3932,7 +3933,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:49" s="4" customFormat="1" ht="79.2">
+    <row r="11" spans="1:49" s="4" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -4081,7 +4082,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:49" s="4" customFormat="1" ht="66">
+    <row r="12" spans="1:49" s="4" customFormat="1" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -4230,7 +4231,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:49" s="4" customFormat="1" ht="19.8">
+    <row r="13" spans="1:49" s="4" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -4379,7 +4380,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:49" s="4" customFormat="1" ht="59.4">
+    <row r="14" spans="1:49" s="4" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -4528,7 +4529,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:49" s="4" customFormat="1" ht="39.6">
+    <row r="15" spans="1:49" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -4677,7 +4678,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:49" s="4" customFormat="1" ht="52.8">
+    <row r="16" spans="1:49" s="4" customFormat="1" ht="59.4" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -4826,7 +4827,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:49" s="4" customFormat="1" ht="19.8">
+    <row r="17" spans="1:49" s="4" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -4975,7 +4976,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:49" s="4" customFormat="1" ht="19.8">
+    <row r="18" spans="1:49" s="4" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -5124,7 +5125,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:49" s="4" customFormat="1" ht="66">
+    <row r="19" spans="1:49" s="4" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -5273,7 +5274,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:49" s="4" customFormat="1" ht="66">
+    <row r="20" spans="1:49" s="4" customFormat="1" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -5422,7 +5423,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:49" s="4" customFormat="1" ht="19.8">
+    <row r="21" spans="1:49" s="4" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -5571,7 +5572,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:49" s="4" customFormat="1" ht="13.2">
+    <row r="22" spans="1:49" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -5720,7 +5721,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:49" s="4" customFormat="1" ht="13.2">
+    <row r="23" spans="1:49" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -5869,7 +5870,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:49" s="4" customFormat="1" ht="409.6">
+    <row r="24" spans="1:49" s="4" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -6018,7 +6019,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="25" spans="1:49" s="4" customFormat="1" ht="99">
+    <row r="25" spans="1:49" s="4" customFormat="1" ht="112.2" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:49" s="4" customFormat="1" ht="105.6">
+    <row r="26" spans="1:49" s="4" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -6316,7 +6317,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="27" spans="1:49" s="4" customFormat="1" ht="19.8">
+    <row r="27" spans="1:49" s="4" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -6465,7 +6466,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="28" spans="1:49" s="4" customFormat="1" ht="85.8">
+    <row r="28" spans="1:49" s="4" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -6614,7 +6615,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:49" s="4" customFormat="1" ht="19.8">
+    <row r="29" spans="1:49" s="4" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -6763,7 +6764,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:49" s="4" customFormat="1" ht="33">
+    <row r="30" spans="1:49" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -6912,7 +6913,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:49" s="4" customFormat="1" ht="6.6">
+    <row r="31" spans="1:49" s="4" customFormat="1" ht="6.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -7061,7 +7062,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="32" spans="1:49" s="4" customFormat="1" ht="6.6">
+    <row r="32" spans="1:49" s="4" customFormat="1" ht="6.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -7210,7 +7211,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="33" spans="1:49" s="4" customFormat="1" ht="19.8">
+    <row r="33" spans="1:49" s="4" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -7359,7 +7360,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="34" spans="1:49" s="4" customFormat="1" ht="79.2">
+    <row r="34" spans="1:49" s="4" customFormat="1" ht="85.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -7508,7 +7509,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:49" s="4" customFormat="1" ht="79.2">
+    <row r="35" spans="1:49" s="4" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -7657,7 +7658,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="36" spans="1:49" s="4" customFormat="1" ht="72.599999999999994">
+    <row r="36" spans="1:49" s="4" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -7806,7 +7807,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:49" s="4" customFormat="1" ht="26.4">
+    <row r="37" spans="1:49" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -7955,7 +7956,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="1:49" s="4" customFormat="1" ht="66">
+    <row r="38" spans="1:49" s="4" customFormat="1" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -8104,7 +8105,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="39" spans="1:49" s="4" customFormat="1" ht="52.8">
+    <row r="39" spans="1:49" s="4" customFormat="1" ht="59.4" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -8253,7 +8254,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:49" s="4" customFormat="1" ht="59.4">
+    <row r="40" spans="1:49" s="4" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -8402,7 +8403,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:49" s="4" customFormat="1" ht="92.4">
+    <row r="41" spans="1:49" s="4" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -8551,7 +8552,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:49" s="4" customFormat="1" ht="46.2">
+    <row r="42" spans="1:49" s="4" customFormat="1" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -8700,7 +8701,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:49" s="4" customFormat="1" ht="39.6">
+    <row r="43" spans="1:49" s="4" customFormat="1" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -8849,7 +8850,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:49" s="4" customFormat="1" ht="39.6">
+    <row r="44" spans="1:49" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -8998,7 +8999,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="45" spans="1:49" s="4" customFormat="1" ht="26.4">
+    <row r="45" spans="1:49" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -9147,7 +9148,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="46" spans="1:49" s="4" customFormat="1" ht="66">
+    <row r="46" spans="1:49" s="4" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -9296,7 +9297,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="47" spans="1:49" s="4" customFormat="1" ht="171.6">
+    <row r="47" spans="1:49" s="4" customFormat="1" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -9445,7 +9446,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="48" spans="1:49" s="4" customFormat="1" ht="92.4">
+    <row r="48" spans="1:49" s="4" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -9594,7 +9595,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="49" spans="1:49" s="4" customFormat="1" ht="105.6">
+    <row r="49" spans="1:49" s="4" customFormat="1" ht="112.2" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -9743,7 +9744,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="50" spans="1:49" s="4" customFormat="1" ht="79.2">
+    <row r="50" spans="1:49" s="4" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -9892,7 +9893,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="51" spans="1:49" s="4" customFormat="1" ht="72.599999999999994">
+    <row r="51" spans="1:49" s="4" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -10041,7 +10042,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="52" spans="1:49" s="4" customFormat="1" ht="79.2">
+    <row r="52" spans="1:49" s="4" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -10190,7 +10191,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="53" spans="1:49" s="4" customFormat="1" ht="118.8">
+    <row r="53" spans="1:49" s="4" customFormat="1" ht="125.4" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -10339,7 +10340,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="54" spans="1:49" s="4" customFormat="1" ht="19.8">
+    <row r="54" spans="1:49" s="4" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -10488,7 +10489,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="55" spans="1:49" s="4" customFormat="1" ht="59.4">
+    <row r="55" spans="1:49" s="4" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -10637,7 +10638,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="56" spans="1:49" s="4" customFormat="1" ht="112.2">
+    <row r="56" spans="1:49" s="4" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -10786,7 +10787,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="57" spans="1:49" s="4" customFormat="1" ht="33">
+    <row r="57" spans="1:49" s="4" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -10935,7 +10936,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="58" spans="1:49" s="4" customFormat="1" ht="105.6">
+    <row r="58" spans="1:49" s="4" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -11084,7 +11085,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="59" spans="1:49" s="4" customFormat="1" ht="39.6">
+    <row r="59" spans="1:49" s="4" customFormat="1" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -11233,7 +11234,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:49" s="4" customFormat="1" ht="178.2">
+    <row r="60" spans="1:49" s="4" customFormat="1" ht="191.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -11382,7 +11383,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:49" s="4" customFormat="1" ht="125.4">
+    <row r="61" spans="1:49" s="4" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -11531,7 +11532,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:49" s="4" customFormat="1" ht="33">
+    <row r="62" spans="1:49" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -11680,7 +11681,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="63" spans="1:49" s="4" customFormat="1" ht="13.2">
+    <row r="63" spans="1:49" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>61</v>
       </c>

</xml_diff>